<commit_message>
ready to submit HW3
</commit_message>
<xml_diff>
--- a/HW/HW2/code/timing.xlsx
+++ b/HW/HW2/code/timing.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7695" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="fig" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>CN</t>
   </si>
@@ -58,6 +62,12 @@
   </si>
   <si>
     <t>slope</t>
+  </si>
+  <si>
+    <t>n_x</t>
+  </si>
+  <si>
+    <t>Log(n_x)</t>
   </si>
 </sst>
 </file>
@@ -148,10 +158,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.4606029485852214E-2"/>
-          <c:y val="9.8459831562401026E-2"/>
-          <c:w val="0.91206111698564463"/>
-          <c:h val="0.87033444869730925"/>
+          <c:x val="0.17319708291340749"/>
+          <c:y val="8.6341911641926616E-2"/>
+          <c:w val="0.79968877885514977"/>
+          <c:h val="0.8824524274568214"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -189,37 +199,34 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$23:$E$28</c:f>
+              <c:f>Sheet1!$M$23:$M$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-1.2041199826559248</c:v>
+                  <c:v>1.2041199826559248</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.505149978319906</c:v>
+                  <c:v>1.505149978319906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.8061799739838871</c:v>
+                  <c:v>1.8061799739838871</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.1072099696478683</c:v>
+                  <c:v>2.1072099696478683</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.4082399653118496</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-2.7092699609758308</c:v>
+                  <c:v>2.4082399653118496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$23:$F$28</c:f>
+              <c:f>Sheet1!$F$23:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>-5.6989700043360205</c:v>
                 </c:pt>
@@ -234,9 +241,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-1.8162178487229388</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.6208286900055916</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,24 +284,24 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$9</c:f>
+              <c:f>Sheet1!$M$5:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-1.2041199826559248</c:v>
+                  <c:v>1.2041199826559248</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.505149978319906</c:v>
+                  <c:v>1.505149978319906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.8061799739838871</c:v>
+                  <c:v>1.8061799739838871</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.1072099696478683</c:v>
+                  <c:v>2.1072099696478683</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.4082399653118496</c:v>
+                  <c:v>2.4082399653118496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -330,6 +334,103 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2AE5-4E5F-84AC-C38BC09BBAA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>ADI</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="50800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[2]Sheet1!$L$22:$L$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2041199826559248</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.505149978319906</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8061799739838871</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1072099696478683</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4082399653118496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7092699609758308</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0102999566398121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[2]Sheet1!$J$22:$J$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>-5.154901959985744</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.6989700043360187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.2441251443275085</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.8927900303521352</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.4282911681913122</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.8236193077567324</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.1756788751492286</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6FC0-4E1C-9EE2-BCCB8A710D4C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -348,7 +449,6 @@
         <c:axId val="429854848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="-1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -374,11 +474,11 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>∆</a:t>
+                  <a:t>Nx</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="3200"/>
-                  <a:t>x)</a:t>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -387,8 +487,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.40307965498341902"/>
-              <c:y val="9.1174132327392302E-3"/>
+              <c:x val="0.46903293060846352"/>
+              <c:y val="1.0387733441727073E-3"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -459,6 +559,7 @@
         <c:axId val="435766520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="-1.5"/>
           <c:min val="-6"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -480,15 +581,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:rPr lang="en-US" sz="3600"/>
                   <a:t>Log(time_</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:rPr lang="en-US" sz="2800"/>
                   <a:t>MSec</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:rPr lang="en-US" sz="3600"/>
                   <a:t>)</a:t>
                 </a:r>
               </a:p>
@@ -498,8 +599,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.93892961078601267"/>
-              <c:y val="0.39432685106482385"/>
+              <c:x val="2.7308362937309965E-2"/>
+              <c:y val="0.32565846493726491"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -580,10 +681,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.44111986001749781"/>
-          <c:y val="0.27340392025464905"/>
-          <c:w val="0.28704243227831633"/>
-          <c:h val="0.21077773079445414"/>
+          <c:x val="0.20193126061066419"/>
+          <c:y val="0.2129436056757863"/>
+          <c:w val="0.40239989262824344"/>
+          <c:h val="0.27405455245757682"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -599,7 +700,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="3200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -1210,7 +1311,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1222,7 +1323,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6293013"/>
+    <xdr:ext cx="8665221" cy="6288186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1249,6 +1350,164 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="err"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="M2">
+            <v>-0.6020599913279624</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="I22">
+            <v>-1.2041199826559248</v>
+          </cell>
+          <cell r="J22">
+            <v>-5.154901959985744</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="I23">
+            <v>-1.505149978319906</v>
+          </cell>
+          <cell r="J23">
+            <v>-4.6989700043360187</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="I24">
+            <v>-1.8061799739838871</v>
+          </cell>
+          <cell r="J24">
+            <v>-4.2441251443275085</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="I25">
+            <v>-2.1072099696478683</v>
+          </cell>
+          <cell r="J25">
+            <v>-3.8927900303521352</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="I26">
+            <v>-2.4082399653118496</v>
+          </cell>
+          <cell r="J26">
+            <v>-3.4282911681913122</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="I27">
+            <v>-2.7092699609758308</v>
+          </cell>
+          <cell r="J27">
+            <v>-2.8236193077567324</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="I28">
+            <v>-3.0102999566398121</v>
+          </cell>
+          <cell r="J28">
+            <v>-2.1756788751492286</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="err"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="1">
+        <row r="20">
+          <cell r="L20">
+            <v>0.6020599913279624</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="L21">
+            <v>0.90308998699194354</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="J22">
+            <v>-5.154901959985744</v>
+          </cell>
+          <cell r="L22">
+            <v>1.2041199826559248</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="J23">
+            <v>-4.6989700043360187</v>
+          </cell>
+          <cell r="L23">
+            <v>1.505149978319906</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="J24">
+            <v>-4.2441251443275085</v>
+          </cell>
+          <cell r="L24">
+            <v>1.8061799739838871</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="J25">
+            <v>-3.8927900303521352</v>
+          </cell>
+          <cell r="L25">
+            <v>2.1072099696478683</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="J26">
+            <v>-3.4282911681913122</v>
+          </cell>
+          <cell r="L26">
+            <v>2.4082399653118496</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="J27">
+            <v>-2.8236193077567324</v>
+          </cell>
+          <cell r="L27">
+            <v>2.7092699609758308</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="J28">
+            <v>-2.1756788751492286</v>
+          </cell>
+          <cell r="L28">
+            <v>3.0102999566398121</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1548,10 +1807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,12 +1820,12 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1594,8 +1853,14 @@
       <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1628,8 +1893,16 @@
         <f>I3/H3</f>
         <v>-3.3659768686032119</v>
       </c>
+      <c r="L3" s="1">
+        <f>1/C3</f>
+        <v>4</v>
+      </c>
+      <c r="M3" s="1">
+        <f>LOG(L3)</f>
+        <v>0.6020599913279624</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1650,8 +1923,16 @@
         <f t="shared" si="0"/>
         <v>#NUM!</v>
       </c>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4:L10" si="1">1/C4</f>
+        <v>8</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M9" si="2">LOG(L4)</f>
+        <v>0.90308998699194354</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1672,8 +1953,16 @@
         <f t="shared" si="0"/>
         <v>-6.0000000000000009</v>
       </c>
+      <c r="L5" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2041199826559248</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1694,8 +1983,16 @@
         <f t="shared" si="0"/>
         <v>-4.9586073148417746</v>
       </c>
+      <c r="L6" s="1">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="2"/>
+        <v>1.505149978319906</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1716,8 +2013,16 @@
         <f t="shared" si="0"/>
         <v>-3.9665762445130541</v>
       </c>
+      <c r="L7" s="1">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8061799739838871</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1738,8 +2043,16 @@
         <f t="shared" si="0"/>
         <v>-3.0803989762158897</v>
       </c>
+      <c r="L8" s="1">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="2"/>
+        <v>2.1072099696478683</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1760,13 +2073,21 @@
         <f t="shared" si="0"/>
         <v>-1.9469599913572573</v>
       </c>
+      <c r="L9" s="1">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4082399653118496</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -1794,8 +2115,14 @@
       <c r="J20" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1828,8 +2155,16 @@
         <f>I21/H21</f>
         <v>-3.2245558678038906</v>
       </c>
+      <c r="L21" s="1">
+        <f>1/C21</f>
+        <v>4</v>
+      </c>
+      <c r="M21" s="1">
+        <f>LOG(L21)</f>
+        <v>0.6020599913279624</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -1843,15 +2178,23 @@
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" ref="E22:F28" si="1">LOG10(C22)</f>
+        <f t="shared" ref="E22:F28" si="3">LOG10(C22)</f>
         <v>-0.90308998699194354</v>
       </c>
       <c r="F22" s="1" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#NUM!</v>
       </c>
+      <c r="L22" s="1">
+        <f t="shared" ref="L22:L28" si="4">1/C22</f>
+        <v>8</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" ref="M22:M28" si="5">LOG(L22)</f>
+        <v>0.90308998699194354</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>3</v>
       </c>
@@ -1865,15 +2208,23 @@
         <v>1.9999999999999902E-6</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-1.2041199826559248</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-5.6989700043360205</v>
       </c>
+      <c r="L23" s="1">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2041199826559248</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>4</v>
       </c>
@@ -1887,15 +2238,23 @@
         <v>6.9999999999999897E-6</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-1.505149978319906</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-5.154901959985744</v>
       </c>
+      <c r="L24" s="1">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="5"/>
+        <v>1.505149978319906</v>
+      </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>5</v>
       </c>
@@ -1909,15 +2268,23 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-1.8061799739838871</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-4.0969100130080562</v>
       </c>
+      <c r="L25" s="1">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="5"/>
+        <v>1.8061799739838871</v>
+      </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -1931,15 +2298,23 @@
         <v>1.047E-3</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-2.1072099696478683</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-2.9800533183211577</v>
       </c>
+      <c r="L26" s="1">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="M26" s="1">
+        <f t="shared" si="5"/>
+        <v>2.1072099696478683</v>
+      </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>7</v>
       </c>
@@ -1953,15 +2328,23 @@
         <v>1.5268E-2</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-2.4082399653118496</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-1.8162178487229388</v>
       </c>
+      <c r="L27" s="1">
+        <f t="shared" si="4"/>
+        <v>256</v>
+      </c>
+      <c r="M27" s="1">
+        <f t="shared" si="5"/>
+        <v>2.4082399653118496</v>
+      </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>8</v>
       </c>
@@ -1975,12 +2358,20 @@
         <v>0.239426</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-2.7092699609758308</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-0.6208286900055916</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="4"/>
+        <v>512</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="5"/>
+        <v>2.7092699609758308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>